<commit_message>
Dodani dijagrami aktivnosti za rezrevacije karata
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/Ukrcavanje.xlsx
+++ b/UseCaseIScenarij/Ukrcavanje.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lejla\Desktop\Scneariji\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lejla\Grupa6-piloti\UseCaseIScenarij\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39,9 +39,6 @@
     <t>1. Prikazuje boarding pass</t>
   </si>
   <si>
-    <t>2. Unos podataka sa boarding pass</t>
-  </si>
-  <si>
     <t>3. Provjeravanje validnosti boarding pass</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>3. Nije dozvoljeno ukrcavanje</t>
+  </si>
+  <si>
+    <t>2. Skenira boarding pass</t>
   </si>
 </sst>
 </file>
@@ -442,19 +442,19 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -547,7 +547,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -555,12 +555,12 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>

</xml_diff>